<commit_message>
feat: add back npc
</commit_message>
<xml_diff>
--- a/npc/NPC性能评估结果.xlsx
+++ b/npc/NPC性能评估结果.xlsx
@@ -99,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,12 +110,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -185,29 +179,29 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,7 +607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="62.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="48">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
fix: 修复ICache使用Vec嵌套无法通过部分参数编译的Bug fix: 修复ICacheTracer统计错误的Bug feat: ICache采用toatal: 64B, block: 32B的参数设计 feat: 添加FENCE.I指令
</commit_message>
<xml_diff>
--- a/npc/NPC性能评估结果.xlsx
+++ b/npc/NPC性能评估结果.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>commit</t>
   </si>
@@ -99,6 +99,34 @@
   </si>
   <si>
     <t>ECALL/EBREAK指令平均执行周期</t>
+  </si>
+  <si>
+    <r>
+      <t>FENCE.I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="文泉驿微米黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指令计数器</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FENCE.I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="文泉驿微米黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指令平均执行周期</t>
+    </r>
   </si>
   <si>
     <t>缓存访问次数</t>
@@ -800,7 +828,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -833,9 +861,6 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,9 +870,6 @@
     <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -860,11 +882,11 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1217,10 +1239,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AF31" sqref="AF31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
@@ -1246,14 +1268,14 @@
     <col min="22" max="22" width="14.5833333333333" style="5" customWidth="1"/>
     <col min="23" max="23" width="14.5833333333333" style="6" customWidth="1"/>
     <col min="24" max="24" width="14.5833333333333" style="5" customWidth="1"/>
-    <col min="25" max="26" width="14.5833333333333" style="6" customWidth="1"/>
-    <col min="27" max="30" width="14.5833333333333" style="7" customWidth="1"/>
-    <col min="31" max="33" width="14.5833333333333" style="8" customWidth="1"/>
-    <col min="34" max="34" width="14.5833333333333" style="4" customWidth="1"/>
-    <col min="35" max="38" width="14.5833333333333" style="9" customWidth="1"/>
+    <col min="25" max="28" width="14.5833333333333" style="6" customWidth="1"/>
+    <col min="29" max="32" width="14.5833333333333" style="7" customWidth="1"/>
+    <col min="33" max="35" width="14.5833333333333" style="8" customWidth="1"/>
+    <col min="36" max="36" width="14.5833333333333" style="4" customWidth="1"/>
+    <col min="37" max="40" width="14.5833333333333" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="50" customHeight="1" spans="1:38">
+    <row r="1" s="1" customFormat="1" ht="50" customHeight="1" spans="1:40">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1266,296 +1288,308 @@
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="13" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="17" t="s">
+      <c r="Y1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AF1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="20" t="s">
+      <c r="AG1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
+      <c r="AH1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="19"/>
       <c r="AK1" s="9"/>
       <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="50" customHeight="1" spans="1:38">
-      <c r="A2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="13" t="s">
+    <row r="2" s="2" customFormat="1" ht="50" customHeight="1" spans="1:40">
+      <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="13">
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="12">
         <v>19926.06</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="3">
         <v>7916089010</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="3">
         <v>196243122</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="3">
         <v>40.34</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="3">
         <v>0.024789</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="3">
         <v>15954862</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2" s="3">
         <v>48.541034</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="3">
         <v>4071016</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="3">
         <v>2</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="3">
         <v>52759794</v>
       </c>
-      <c r="N2" s="16">
+      <c r="N2" s="3">
         <v>2</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="3">
         <v>15954862</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="3">
         <v>52.541034</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2" s="3">
         <v>7241375</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2" s="3">
         <v>28.286903</v>
       </c>
-      <c r="S2" s="16">
+      <c r="S2" s="3">
         <v>116216072</v>
       </c>
-      <c r="T2" s="16">
+      <c r="T2" s="3">
         <v>2</v>
       </c>
-      <c r="U2" s="16">
+      <c r="U2" s="3">
         <v>2</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="3">
         <v>2</v>
       </c>
-      <c r="W2" s="16">
+      <c r="W2" s="3">
         <v>1</v>
       </c>
-      <c r="X2" s="16">
+      <c r="X2" s="3">
         <v>2</v>
       </c>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="21">
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="20">
         <f>($K2*$L2+$M2*$N2+$O2*$P2+$Q2*$R2+$S2*$T2+$U2*$V2+$W2*$X2)/$F2</f>
         <v>7.07904957310521</v>
       </c>
-      <c r="AG2" s="21">
-        <f>$G2-$AF2</f>
+      <c r="AI2" s="20">
+        <f>$G2-$AH2</f>
         <v>33.2609504268948</v>
       </c>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
     </row>
-    <row r="3" s="2" customFormat="1" ht="50" customHeight="1" spans="1:38">
-      <c r="A3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="13" t="s">
+    <row r="3" s="2" customFormat="1" ht="50" customHeight="1" spans="1:40">
+      <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="13">
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="12">
         <v>31364.858</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="3">
         <v>3664478516</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="3">
         <v>196237829</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="3">
         <v>18.67366</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="3">
         <v>0.053551</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="3">
         <v>15954592</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="3">
         <v>46.696262</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="3">
         <v>4070935</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="3">
         <v>2</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="3">
         <v>52759602</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="3">
         <v>2</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="3">
         <v>15954592</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="3">
         <v>49.696262</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="3">
         <v>7241117</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="3">
         <v>26.386494</v>
       </c>
-      <c r="S3" s="16">
+      <c r="S3" s="3">
         <v>116211580</v>
       </c>
-      <c r="T3" s="16">
+      <c r="T3" s="3">
         <v>2</v>
       </c>
-      <c r="U3" s="16">
+      <c r="U3" s="3">
         <v>2</v>
       </c>
-      <c r="V3" s="16">
+      <c r="V3" s="3">
         <v>2</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="3">
         <v>1</v>
       </c>
-      <c r="X3" s="16">
+      <c r="X3" s="3">
         <v>2</v>
       </c>
-      <c r="Y3" s="16">
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3">
         <v>196042461</v>
       </c>
-      <c r="Z3" s="16">
+      <c r="AB3" s="3">
         <v>145706428</v>
       </c>
-      <c r="AA3" s="16">
+      <c r="AC3" s="3">
         <v>74.323913</v>
       </c>
-      <c r="AB3" s="16">
+      <c r="AD3" s="3">
         <v>2.256761</v>
       </c>
-      <c r="AC3" s="16">
+      <c r="AE3" s="3">
         <v>33.669864</v>
       </c>
-      <c r="AD3" s="16">
+      <c r="AF3" s="3">
         <v>10.901864</v>
       </c>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="21">
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="20">
         <f>($K3*$L3+$M3*$N3+$O3*$P3+$Q3*$R3+$S3*$T3+$U3*$V3+$W3*$X3)/$F3</f>
         <v>6.77767136533549</v>
       </c>
-      <c r="AG3" s="21">
-        <f>$G3-$AF3</f>
+      <c r="AI3" s="20">
+        <f>$G3-$AH3</f>
         <v>11.8959886346645</v>
       </c>
-      <c r="AI3" s="23"/>
-      <c r="AJ3" s="23"/>
-      <c r="AK3" s="23"/>
-      <c r="AL3" s="23"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>